<commit_message>
update single neuron data
</commit_message>
<xml_diff>
--- a/data_2nd_round/Supplementary Table 1_plusNewData.xlsx
+++ b/data_2nd_round/Supplementary Table 1_plusNewData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab Admin\Documents\GitHub\larval_olfaction\data_2nd_round\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="45" windowWidth="24720" windowHeight="12330"/>
+    <workbookView xWindow="2340" yWindow="45" windowWidth="24720" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3854" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3867" uniqueCount="189">
   <si>
     <t>Odor</t>
   </si>
@@ -563,11 +568,32 @@
   <si>
     <t>NaN</t>
   </si>
+  <si>
+    <t>run101_L</t>
+  </si>
+  <si>
+    <t>run102_L</t>
+  </si>
+  <si>
+    <t>run103_L</t>
+  </si>
+  <si>
+    <t>run104_L</t>
+  </si>
+  <si>
+    <t>run105_L</t>
+  </si>
+  <si>
+    <t>run106_L</t>
+  </si>
+  <si>
+    <t>or22c/methyl salicylate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -616,6 +642,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +703,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -709,9 +736,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -744,6 +788,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -922,9 +983,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1194" sqref="AC1194"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A784" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C789" sqref="C789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -89451,12 +89512,264 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="B2">
+        <v>0.52836271698369297</v>
+      </c>
+      <c r="C2">
+        <v>0.101782387178684</v>
+      </c>
+      <c r="D2">
+        <v>0.163262441014592</v>
+      </c>
+      <c r="E2">
+        <v>0.138902424753691</v>
+      </c>
+      <c r="F2">
+        <v>1.4536215482678699E-3</v>
+      </c>
+      <c r="G2">
+        <v>8.1214879452363803E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.1584424374458</v>
+      </c>
+      <c r="I2">
+        <v>0.14453199566029501</v>
+      </c>
+      <c r="J2">
+        <v>0.11292618810242901</v>
+      </c>
+      <c r="K2">
+        <v>4.2030761854306098E-2</v>
+      </c>
+      <c r="L2">
+        <v>0.145080415488022</v>
+      </c>
+      <c r="M2">
+        <v>0.156447348810547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1E-10</v>
+      </c>
+      <c r="B3">
+        <v>0.55738437434600896</v>
+      </c>
+      <c r="C3">
+        <v>0.16982417956877599</v>
+      </c>
+      <c r="D3">
+        <v>0.30019167571563199</v>
+      </c>
+      <c r="E3">
+        <v>0.25639373123536102</v>
+      </c>
+      <c r="F3">
+        <v>3.94607485036612E-2</v>
+      </c>
+      <c r="G3">
+        <v>5.8946101478165799E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.163754168517383</v>
+      </c>
+      <c r="I3">
+        <v>0.319183381538856</v>
+      </c>
+      <c r="J3">
+        <v>0.17069586700829001</v>
+      </c>
+      <c r="K3">
+        <v>-1.6782425283383601E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.279855673684275</v>
+      </c>
+      <c r="M3">
+        <v>0.18799793637145301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="B4">
+        <v>3.5776107330923801</v>
+      </c>
+      <c r="C4">
+        <v>1.2718703798358899</v>
+      </c>
+      <c r="D4">
+        <v>3.5990539413856202</v>
+      </c>
+      <c r="E4">
+        <v>2.3572158385337301</v>
+      </c>
+      <c r="F4">
+        <v>1.1248387272515701</v>
+      </c>
+      <c r="G4">
+        <v>0.89961785835182595</v>
+      </c>
+      <c r="H4">
+        <v>1.3958572163821901</v>
+      </c>
+      <c r="I4">
+        <v>1.32720217081911</v>
+      </c>
+      <c r="J4">
+        <v>1.18801188882945</v>
+      </c>
+      <c r="K4">
+        <v>7.6278099658679804E-3</v>
+      </c>
+      <c r="L4">
+        <v>1.4207256988296599</v>
+      </c>
+      <c r="M4">
+        <v>0.99578928059615901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1E-8</v>
+      </c>
+      <c r="B5">
+        <v>5.2116527808415203</v>
+      </c>
+      <c r="C5">
+        <v>5.1916712009541204</v>
+      </c>
+      <c r="D5">
+        <v>5.0905030269864504</v>
+      </c>
+      <c r="E5">
+        <v>5.8322827755683804</v>
+      </c>
+      <c r="F5">
+        <v>4.7273066646195501</v>
+      </c>
+      <c r="G5">
+        <v>5.5138616617143699</v>
+      </c>
+      <c r="H5">
+        <v>3.0354153006620299</v>
+      </c>
+      <c r="I5">
+        <v>4.7942032557454004</v>
+      </c>
+      <c r="J5">
+        <v>4.3625229211719798</v>
+      </c>
+      <c r="K5">
+        <v>0.94403449231827896</v>
+      </c>
+      <c r="L5">
+        <v>3.79620453908707</v>
+      </c>
+      <c r="M5">
+        <v>4.7312220120378301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B6">
+        <v>5.89851752555162</v>
+      </c>
+      <c r="C6">
+        <v>5.2090279037302096</v>
+      </c>
+      <c r="D6">
+        <v>5.1950565429035596</v>
+      </c>
+      <c r="E6">
+        <v>5.7251695476226701</v>
+      </c>
+      <c r="F6">
+        <v>4.72077465399102</v>
+      </c>
+      <c r="G6">
+        <v>5.4607703012750601</v>
+      </c>
+      <c r="H6">
+        <v>2.5322969323942299</v>
+      </c>
+      <c r="I6">
+        <v>4.4062693758411804</v>
+      </c>
+      <c r="J6">
+        <v>4.2907976047505398</v>
+      </c>
+      <c r="K6">
+        <v>4.09372649882493</v>
+      </c>
+      <c r="L6">
+        <v>3.7320100511723</v>
+      </c>
+      <c r="M6">
+        <v>4.5589869876755502</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>